<commit_message>
additions of code and notebooks
</commit_message>
<xml_diff>
--- a/data/fluorimeter/AAN155__EMISSION_1E-5.xlsx
+++ b/data/fluorimeter/AAN155__EMISSION_1E-5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/JuliaProjects/LaserLab/data/fluorimeter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0476FBDD-C253-6442-A4D0-C6C25B513D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{965FF528-9039-B148-B9A0-BDBB02791B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5060" yWindow="1520" windowWidth="34320" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20180" yWindow="1820" windowWidth="34320" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AAN155__EMISSION_1E-5" sheetId="1" r:id="rId1"/>

</xml_diff>